<commit_message>
Update 27-08-2016 Hoàn thành sản phẩm
Test chức năng, tạo file cài đặt, fix bug
</commit_message>
<xml_diff>
--- a/AppSendMailMakerting/Resources/KhachHang.xlsx
+++ b/AppSendMailMakerting/Resources/KhachHang.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Email</t>
   </si>
@@ -32,6 +32,54 @@
   </si>
   <si>
     <t>Lokit007</t>
+  </si>
+  <si>
+    <t>lokit.ho.14@facebook.com</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>ditimhacker@gmail.com</t>
+  </si>
+  <si>
+    <t>fshare@sinhvienit.net</t>
+  </si>
+  <si>
+    <t>11t3minhquang@gmail.com</t>
+  </si>
+  <si>
+    <t>congthongtin.vietnhat@gmail.com</t>
+  </si>
+  <si>
+    <t>tuanvubkt3@gmail.com</t>
+  </si>
+  <si>
+    <t>vinhbietsinhvien@gmail.com</t>
+  </si>
+  <si>
+    <t>bkwoodroot@gmail.com</t>
+  </si>
+  <si>
+    <t>Bkwood</t>
+  </si>
+  <si>
+    <t>sinhvien</t>
+  </si>
+  <si>
+    <t>tuanvu</t>
+  </si>
+  <si>
+    <t>thong tin viet nhat</t>
+  </si>
+  <si>
+    <t>minh quang</t>
+  </si>
+  <si>
+    <t>fshared</t>
+  </si>
+  <si>
+    <t>hacker</t>
   </si>
 </sst>
 </file>
@@ -400,11 +448,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,10 +485,82 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>